<commit_message>
politiezone aalter + refreg
</commit_message>
<xml_diff>
--- a/data_voor_swing/aggregatietabellen/gemeente_refreg.xlsx
+++ b/data_voor_swing/aggregatietabellen/gemeente_refreg.xlsx
@@ -420,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B303"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,7 +663,7 @@
         <v>11056</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>